<commit_message>
second commit: Project with library dependencies
</commit_message>
<xml_diff>
--- a/my_data.xlsx
+++ b/my_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,160 +466,12 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Show me basketball highlights from yesterday"</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>basketball</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>highlights</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>yesterday</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>"Find MMA news regarding the next title fight"</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>mma</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>news</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>"What are the live football matches today?"</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>football</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>matches</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>today</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>"Show me upcoming soccer matches next week"</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>football</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>matches</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>next week</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>"Find basketball analysis of the Lakers game"</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>basketball</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>analysis</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>"Show me a preview of the UFC 300 card"</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>mma</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>preview</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>me a</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>"Find football highlights from last week"</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>football</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>highlights</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>